<commit_message>
Deepthi - First Test case - View Licence Details
</commit_message>
<xml_diff>
--- a/src/main/resources/dataSheets/testData.xlsx
+++ b/src/main/resources/dataSheets/testData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AvoComp14\Documents\dlp-automation\src\main\resources\dataSheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AvoComp13\Documents\dlp-automation\src\main\resources\dataSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23325" windowHeight="7770"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23325" windowHeight="7770" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="devices" sheetId="19" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>deviceName</t>
   </si>
@@ -85,6 +85,15 @@
   </si>
   <si>
     <t>au.gov.nsw.onegov.app.holder.uat</t>
+  </si>
+  <si>
+    <t>PIN</t>
+  </si>
+  <si>
+    <t>LicenceNumber</t>
+  </si>
+  <si>
+    <t>LicenceName</t>
   </si>
 </sst>
 </file>
@@ -412,7 +421,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
@@ -489,32 +498,47 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B2" t="s">
         <v>17</v>
+      </c>
+      <c r="C2">
+        <v>1234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DS - Fluentwait added to all Pg Obj
</commit_message>
<xml_diff>
--- a/src/main/resources/dataSheets/testData.xlsx
+++ b/src/main/resources/dataSheets/testData.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16828"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -15,7 +15,7 @@
     <sheet name="devices" sheetId="19" r:id="rId1"/>
     <sheet name="signIn" sheetId="18" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>deviceName</t>
   </si>
@@ -75,31 +75,55 @@
     <t>Android</t>
   </si>
   <si>
+    <t>srirupa.alapati@service.nsw.gov.au</t>
+  </si>
+  <si>
+    <t>Test1234$</t>
+  </si>
+  <si>
+    <t>au.gov.nsw.onegov.app.holder.uat</t>
+  </si>
+  <si>
+    <t>PIN</t>
+  </si>
+  <si>
+    <t>Licence_Number</t>
+  </si>
+  <si>
+    <t>Licence_StartDate</t>
+  </si>
+  <si>
+    <t>Licence_ExpireDate</t>
+  </si>
+  <si>
+    <t>09-12-2013</t>
+  </si>
+  <si>
+    <t>08-12-2016</t>
+  </si>
+  <si>
+    <t>RO4447865</t>
+  </si>
+  <si>
+    <t>class_Type</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
     <t>PerfectoMobile</t>
   </si>
   <si>
-    <t>srirupa.alapati@service.nsw.gov.au</t>
-  </si>
-  <si>
-    <t>Test1234$</t>
-  </si>
-  <si>
-    <t>au.gov.nsw.onegov.app.holder.uat</t>
-  </si>
-  <si>
-    <t>PIN</t>
-  </si>
-  <si>
-    <t>LicenceNumber</t>
-  </si>
-  <si>
-    <t>LicenceName</t>
+    <t>Galaxy S7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -135,10 +159,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,17 +446,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="26.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -483,11 +508,14 @@
       <c r="B2" t="s">
         <v>14</v>
       </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
       <c r="K2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="L2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -498,22 +526,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -521,27 +551,46 @@
         <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
         <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
       </c>
       <c r="C2">
         <v>1234</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
common function on driver page
</commit_message>
<xml_diff>
--- a/src/main/resources/dataSheets/testData.xlsx
+++ b/src/main/resources/dataSheets/testData.xlsx
@@ -5,15 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AvoComp13\Documents\dlp-automation\src\main\resources\dataSheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AvoComp14\Documents\dlp-automation\src\main\resources\dataSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23325" windowHeight="7770"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23325" windowHeight="7770" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="devices" sheetId="19" r:id="rId1"/>
-    <sheet name="signIn" sheetId="18" r:id="rId2"/>
+    <sheet name="checkerapp" sheetId="20" r:id="rId2"/>
+    <sheet name="checkerSignIn" sheetId="21" r:id="rId3"/>
+    <sheet name="signIn" sheetId="18" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="38">
   <si>
     <t>deviceName</t>
   </si>
@@ -81,9 +83,6 @@
     <t>Test1234$</t>
   </si>
   <si>
-    <t>au.gov.nsw.onegov.app.holder.uat</t>
-  </si>
-  <si>
     <t>PIN</t>
   </si>
   <si>
@@ -114,9 +113,6 @@
     <t>09-12-2016</t>
   </si>
   <si>
-    <t>Galaxy S7</t>
-  </si>
-  <si>
     <t>licence_Name</t>
   </si>
   <si>
@@ -127,6 +123,27 @@
   </si>
   <si>
     <t>Check</t>
+  </si>
+  <si>
+    <t>au.gov.nsw.onegov.app.checker.uat</t>
+  </si>
+  <si>
+    <t>DPI-DLTEST</t>
+  </si>
+  <si>
+    <t>SNSW-1234</t>
+  </si>
+  <si>
+    <t>pin</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>Galaxy S7 Edge</t>
+  </si>
+  <si>
+    <t>appName</t>
   </si>
 </sst>
 </file>
@@ -171,11 +188,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,8 +476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,13 +539,13 @@
         <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="K2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -538,10 +556,135 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" customWidth="1"/>
+    <col min="12" max="12" width="37.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="42.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1"/>
+    <col min="4" max="4" width="32.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,25 +708,25 @@
         <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -597,22 +740,22 @@
         <v>1234</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" t="s">
         <v>30</v>
-      </c>
-      <c r="I2" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DS - Renew,Share,Update Lic
</commit_message>
<xml_diff>
--- a/src/main/resources/dataSheets/testData.xlsx
+++ b/src/main/resources/dataSheets/testData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23325" windowHeight="7770"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23325" windowHeight="7770" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="devices" sheetId="19" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>deviceName</t>
   </si>
@@ -127,6 +127,12 @@
   </si>
   <si>
     <t>Check</t>
+  </si>
+  <si>
+    <t>postal_Address</t>
+  </si>
+  <si>
+    <t>2-6 MAWSON</t>
   </si>
 </sst>
 </file>
@@ -171,11 +177,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,7 +465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
@@ -538,10 +545,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,9 +562,10 @@
     <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="45.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -585,8 +593,11 @@
       <c r="I1" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
@@ -613,6 +624,9 @@
       </c>
       <c r="I2" t="s">
         <v>32</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
checker changes are done
</commit_message>
<xml_diff>
--- a/src/main/resources/dataSheets/testData.xlsx
+++ b/src/main/resources/dataSheets/testData.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23325" windowHeight="7770" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23325" windowHeight="7770"/>
   </bookViews>
   <sheets>
     <sheet name="devices" sheetId="19" r:id="rId1"/>
     <sheet name="signIn" sheetId="18" r:id="rId2"/>
     <sheet name="checkerSignIn" sheetId="20" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -115,9 +115,6 @@
     <t>09-12-2016</t>
   </si>
   <si>
-    <t>Galaxy S7</t>
-  </si>
-  <si>
     <t>licence_Name</t>
   </si>
   <si>
@@ -188,6 +185,9 @@
   </si>
   <si>
     <t>2-24 Rawson Pl, HAYMARKET, NSW 2000</t>
+  </si>
+  <si>
+    <t>Galaxy Note5</t>
   </si>
 </sst>
 </file>
@@ -520,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,13 +583,13 @@
         <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="K2" t="s">
         <v>22</v>
       </c>
       <c r="L2" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -644,19 +644,19 @@
         <v>20</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -682,10 +682,10 @@
         <v>21</v>
       </c>
       <c r="H2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J2">
         <v>2222</v>
@@ -694,7 +694,7 @@
         <v>17</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -707,11 +707,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="38.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="8" width="12.140625" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" customWidth="1"/>
+    <col min="12" max="12" width="11" customWidth="1"/>
+    <col min="13" max="13" width="37.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -721,19 +734,19 @@
         <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>23</v>
@@ -745,54 +758,54 @@
         <v>20</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
         <v>43</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" t="s">
         <v>45</v>
-      </c>
-      <c r="D2" t="s">
-        <v>46</v>
       </c>
       <c r="E2" t="s">
         <v>19</v>
       </c>
       <c r="F2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" t="s">
         <v>47</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="J2" t="s">
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
appPackage removed from signIn and checkerSignIn sheets
</commit_message>
<xml_diff>
--- a/src/main/resources/dataSheets/testData.xlsx
+++ b/src/main/resources/dataSheets/testData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AvoComp13\Documents\dlp-automation\src\main\resources\dataSheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AvoComp14\Documents\dlp-automation\src\main\resources\dataSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="51">
   <si>
     <t>deviceName</t>
   </si>
@@ -88,9 +88,6 @@
     <t>General</t>
   </si>
   <si>
-    <t>PerfectoMobile</t>
-  </si>
-  <si>
     <t>licence_StartDate</t>
   </si>
   <si>
@@ -118,9 +115,6 @@
     <t>newPIN</t>
   </si>
   <si>
-    <t>appName</t>
-  </si>
-  <si>
     <t>pin</t>
   </si>
   <si>
@@ -169,15 +163,6 @@
     <t>2-24 Rawson Pl, HAYMARKET, NSW 2000</t>
   </si>
   <si>
-    <t>iPhone-6S Plus</t>
-  </si>
-  <si>
-    <t>iOS</t>
-  </si>
-  <si>
-    <t>au.gov.nsw.onegov.MyLicences.uat</t>
-  </si>
-  <si>
     <t>bundleId</t>
   </si>
   <si>
@@ -194,6 +179,9 @@
   </si>
   <si>
     <t>appPackage</t>
+  </si>
+  <si>
+    <t>Android</t>
   </si>
 </sst>
 </file>
@@ -526,8 +514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,24 +570,18 @@
         <v>9</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" t="s">
-        <v>46</v>
-      </c>
-      <c r="K2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" t="s">
-        <v>48</v>
+        <v>50</v>
+      </c>
+      <c r="M2" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -610,10 +592,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,12 +610,11 @@
     <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -644,37 +625,34 @@
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -688,31 +666,28 @@
         <v>16</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="G2" t="s">
         <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J2">
         <v>2222</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="L2" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="M2" t="s">
-        <v>40</v>
+      <c r="L2" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -723,10 +698,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,19 +709,18 @@
     <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="36.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -754,78 +728,72 @@
         <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>20</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="K2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="L2" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="J2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
automation name missing in capabilities
</commit_message>
<xml_diff>
--- a/src/main/resources/dataSheets/testData.xlsx
+++ b/src/main/resources/dataSheets/testData.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="52">
   <si>
     <t>deviceName</t>
   </si>
@@ -182,6 +182,9 @@
   </si>
   <si>
     <t>Android</t>
+  </si>
+  <si>
+    <t>PerfectoMobile</t>
   </si>
 </sst>
 </file>
@@ -515,7 +518,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,6 +582,9 @@
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>50</v>
+      </c>
+      <c r="K2" t="s">
+        <v>51</v>
       </c>
       <c r="M2" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
scrpit updates regarding clean up and close
</commit_message>
<xml_diff>
--- a/src/main/resources/dataSheets/testData.xlsx
+++ b/src/main/resources/dataSheets/testData.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17030"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23325" windowHeight="7770"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="5955"/>
   </bookViews>
   <sheets>
     <sheet name="devices" sheetId="19" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="73">
   <si>
     <t>deviceName</t>
   </si>
@@ -70,9 +70,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>srirupa.alapati@service.nsw.gov.au</t>
-  </si>
-  <si>
     <t>PIN</t>
   </si>
   <si>
@@ -160,40 +157,97 @@
     <t>bundleId</t>
   </si>
   <si>
-    <t>10 Dec 2013</t>
-  </si>
-  <si>
     <t>lic_OwnerName</t>
   </si>
   <si>
-    <t>9 Dec 2016</t>
-  </si>
-  <si>
-    <t>2 Rawson Avenue, BEXLEY  NSW  2207 AUSTRALIA</t>
-  </si>
-  <si>
     <t>appPackage</t>
   </si>
   <si>
     <t>PerfectoMobile</t>
   </si>
   <si>
-    <t>au.gov.nsw.onegov.LicenceChecker.uat</t>
-  </si>
-  <si>
-    <t>au.gov.nsw.onegov.app.checker.uat</t>
+    <t>cardExpiryMonth</t>
+  </si>
+  <si>
+    <t>cardNumber</t>
+  </si>
+  <si>
+    <t>cardExpiryYear</t>
+  </si>
+  <si>
+    <t>cardCVVNum</t>
+  </si>
+  <si>
+    <t>cardName</t>
+  </si>
+  <si>
+    <t>5163200000000008</t>
+  </si>
+  <si>
+    <t>070</t>
+  </si>
+  <si>
+    <t>2020</t>
+  </si>
+  <si>
+    <t>08-Aug</t>
+  </si>
+  <si>
+    <t>Srikanth</t>
+  </si>
+  <si>
+    <t>au.gov.nsw.onegov.MyLicences.uat</t>
+  </si>
+  <si>
+    <t>appVersion</t>
+  </si>
+  <si>
+    <t>appBuildName</t>
+  </si>
+  <si>
+    <t>automation_psm02@yopmail.com</t>
+  </si>
+  <si>
+    <t>Pa$$w0rd</t>
+  </si>
+  <si>
+    <t>RS2694206</t>
+  </si>
+  <si>
+    <t>08 Aug 2013</t>
   </si>
   <si>
     <t>2222</t>
   </si>
   <si>
-    <t>Pa$$w0rd</t>
-  </si>
-  <si>
-    <t>Android</t>
-  </si>
-  <si>
-    <t>Galaxy S7 Edge</t>
+    <t>2-24 Rawson Pl,HAYMARKET,NSW 2000</t>
+  </si>
+  <si>
+    <t>Jacky Williams</t>
+  </si>
+  <si>
+    <t>1.0.2-PSM</t>
+  </si>
+  <si>
+    <t>au.gov.nsw.onegov.app.holder.psm</t>
+  </si>
+  <si>
+    <t>iOS</t>
+  </si>
+  <si>
+    <t>UAT Holder</t>
+  </si>
+  <si>
+    <t>buildName</t>
+  </si>
+  <si>
+    <t>UAT Checker</t>
+  </si>
+  <si>
+    <t>08 Aug 2017</t>
+  </si>
+  <si>
+    <t>iPhone-6</t>
   </si>
 </sst>
 </file>
@@ -238,15 +292,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -546,8 +599,8 @@
     <col min="9" max="9" width="16" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="36.7109375" customWidth="1"/>
-    <col min="13" max="13" width="39.5703125" customWidth="1"/>
+    <col min="12" max="12" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -585,27 +638,27 @@
         <v>9</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>54</v>
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" t="s">
+        <v>72</v>
       </c>
       <c r="K2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="L2" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="M2" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -616,29 +669,36 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.28515625" customWidth="1"/>
-    <col min="12" max="12" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.42578125" customWidth="1"/>
+    <col min="19" max="19" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -646,72 +706,114 @@
         <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H2" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I2" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="J2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K2" t="s">
+        <v>63</v>
+      </c>
+      <c r="L2" t="s">
+        <v>64</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="O2" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="K2" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="L2" t="s">
-        <v>36</v>
+      <c r="Q2" t="s">
+        <v>54</v>
+      </c>
+      <c r="R2" t="s">
+        <v>68</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -722,10 +824,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,7 +846,7 @@
     <col min="12" max="12" width="36.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -752,72 +854,78 @@
         <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J2" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="K2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="L2" s="4" t="s">
-        <v>41</v>
+      <c r="M2" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Maintained all Holder scripts for data driver
</commit_message>
<xml_diff>
--- a/src/main/resources/dataSheets/testData.xlsx
+++ b/src/main/resources/dataSheets/testData.xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AvoComp14\Documents\dlp-automation\src\main\resources\dataSheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AvoComp13\Documents\dlp-automation\src\main\resources\dataSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="5955"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13605" windowHeight="2115" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="devices" sheetId="19" r:id="rId1"/>
     <sheet name="signIn" sheetId="18" r:id="rId2"/>
     <sheet name="checkerSignIn" sheetId="20" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="91">
   <si>
     <t>deviceName</t>
   </si>
@@ -199,55 +199,109 @@
     <t>au.gov.nsw.onegov.MyLicences.uat</t>
   </si>
   <si>
+    <t>appBuildName</t>
+  </si>
+  <si>
+    <t>2222</t>
+  </si>
+  <si>
+    <t>2-24 Rawson Pl,HAYMARKET,NSW 2000</t>
+  </si>
+  <si>
+    <t>buildName</t>
+  </si>
+  <si>
+    <t>UAT Checker</t>
+  </si>
+  <si>
+    <t>NSW Recreational Fishing Fee</t>
+  </si>
+  <si>
+    <t>Empty</t>
+  </si>
+  <si>
+    <t>windTunnelPersona</t>
+  </si>
+  <si>
+    <t>au.gov.nsw.onegov.app.holder.psm</t>
+  </si>
+  <si>
+    <t>Android</t>
+  </si>
+  <si>
+    <t>PSM Holder</t>
+  </si>
+  <si>
+    <t>Galaxy S7</t>
+  </si>
+  <si>
+    <t>psmtest13@yopmail.com</t>
+  </si>
+  <si>
+    <t>test123</t>
+  </si>
+  <si>
+    <t>Guy Anthony CALLAGHAN</t>
+  </si>
+  <si>
+    <t>RO4128668</t>
+  </si>
+  <si>
+    <t>20 Oct 2015</t>
+  </si>
+  <si>
+    <t>Alanna Scott</t>
+  </si>
+  <si>
+    <t>CCH10011131</t>
+  </si>
+  <si>
+    <t>09 May 2011</t>
+  </si>
+  <si>
+    <t>09 May 2016</t>
+  </si>
+  <si>
+    <t>Liquor &amp; Gaming NSW Competency</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>20 Oct 2016</t>
+  </si>
+  <si>
+    <t>quickView_LicNum</t>
+  </si>
+  <si>
+    <t>CCH######31</t>
+  </si>
+  <si>
+    <t>RO#####68</t>
+  </si>
+  <si>
+    <t>quickView_LicStatus</t>
+  </si>
+  <si>
+    <t>Expired</t>
+  </si>
+  <si>
     <t>appVersion</t>
   </si>
   <si>
-    <t>appBuildName</t>
-  </si>
-  <si>
-    <t>automation_psm02@yopmail.com</t>
-  </si>
-  <si>
-    <t>Pa$$w0rd</t>
-  </si>
-  <si>
-    <t>RS2694206</t>
-  </si>
-  <si>
-    <t>08 Aug 2013</t>
-  </si>
-  <si>
-    <t>2222</t>
-  </si>
-  <si>
-    <t>2-24 Rawson Pl,HAYMARKET,NSW 2000</t>
-  </si>
-  <si>
-    <t>Jacky Williams</t>
-  </si>
-  <si>
-    <t>1.0.2-PSM</t>
-  </si>
-  <si>
-    <t>au.gov.nsw.onegov.app.holder.psm</t>
-  </si>
-  <si>
-    <t>iOS</t>
-  </si>
-  <si>
-    <t>UAT Holder</t>
-  </si>
-  <si>
-    <t>buildName</t>
-  </si>
-  <si>
-    <t>UAT Checker</t>
-  </si>
-  <si>
-    <t>08 Aug 2017</t>
-  </si>
-  <si>
-    <t>iPhone-6</t>
+    <t>activity_LicType</t>
+  </si>
+  <si>
+    <t>Competency Card</t>
+  </si>
+  <si>
+    <t>activity_EventType</t>
+  </si>
+  <si>
+    <t>Add</t>
+  </si>
+  <si>
+    <t>Recreational Fishing</t>
   </si>
 </sst>
 </file>
@@ -257,10 +311,33 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -289,19 +366,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -582,8 +666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,10 +730,10 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" t="s">
         <v>67</v>
-      </c>
-      <c r="E2" t="s">
-        <v>72</v>
       </c>
       <c r="K2" t="s">
         <v>44</v>
@@ -658,7 +742,7 @@
         <v>55</v>
       </c>
       <c r="M2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -669,165 +753,241 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.42578125" customWidth="1"/>
-    <col min="19" max="19" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.5703125" style="7" customWidth="1"/>
+    <col min="20" max="20" width="15.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17" style="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="20.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="16.5703125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="R1" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="J2" s="10">
+        <v>2222</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="T2" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="U2" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="V2" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="W2" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="K3" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="K2" t="s">
-        <v>63</v>
-      </c>
-      <c r="L2" t="s">
-        <v>64</v>
-      </c>
-      <c r="M2" s="4" t="s">
+      <c r="L3" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="M3" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N3" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O3" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P3" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q3" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="R2" t="s">
-        <v>68</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>65</v>
+      <c r="R3" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="T3" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="U3" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="V3" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="W3" s="7" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -844,9 +1004,11 @@
     <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -884,10 +1046,13 @@
         <v>31</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>69</v>
+        <v>59</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>32</v>
       </c>
@@ -925,7 +1090,10 @@
         <v>40</v>
       </c>
       <c r="M2" t="s">
-        <v>70</v>
+        <v>60</v>
+      </c>
+      <c r="N2" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Activity Test Case Changes
</commit_message>
<xml_diff>
--- a/src/main/resources/dataSheets/testData.xlsx
+++ b/src/main/resources/dataSheets/testData.xlsx
@@ -232,9 +232,6 @@
     <t>PSM Holder</t>
   </si>
   <si>
-    <t>Galaxy S7</t>
-  </si>
-  <si>
     <t>psmtest13@yopmail.com</t>
   </si>
   <si>
@@ -302,6 +299,9 @@
   </si>
   <si>
     <t>Recreational Fishing</t>
+  </si>
+  <si>
+    <t>Galaxy Note5</t>
   </si>
 </sst>
 </file>
@@ -667,7 +667,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,7 +733,7 @@
         <v>65</v>
       </c>
       <c r="E2" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="K2" t="s">
         <v>44</v>
@@ -755,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="W2" sqref="W2"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -842,63 +842,63 @@
         <v>56</v>
       </c>
       <c r="S1" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="V1" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="T1" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="W1" s="7" t="s">
-        <v>88</v>
+      <c r="W1" s="5" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>68</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>69</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>34</v>
       </c>
       <c r="D2" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="F2" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="G2" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>76</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>77</v>
       </c>
       <c r="J2" s="10">
         <v>2222</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="R2" s="7" t="s">
         <v>66</v>
       </c>
       <c r="T2" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="U2" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="V2" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="W2" s="7" t="s">
         <v>23</v>
@@ -906,22 +906,22 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>68</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>69</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>34</v>
       </c>
       <c r="D3" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="E3" s="9" t="s">
-        <v>72</v>
-      </c>
       <c r="F3" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>16</v>
@@ -939,7 +939,7 @@
         <v>58</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M3" s="9" t="s">
         <v>50</v>
@@ -960,16 +960,16 @@
         <v>66</v>
       </c>
       <c r="T3" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="U3" s="9" t="s">
         <v>36</v>
       </c>
       <c r="V3" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="W3" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DLP Mobile Automation first commit
</commit_message>
<xml_diff>
--- a/src/main/resources/dataSheets/testData.xlsx
+++ b/src/main/resources/dataSheets/testData.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17030"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13605" windowHeight="2115" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13605" windowHeight="2115"/>
   </bookViews>
   <sheets>
     <sheet name="devices" sheetId="19" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="72">
   <si>
     <t>deviceName</t>
   </si>
@@ -163,9 +163,6 @@
     <t>appPackage</t>
   </si>
   <si>
-    <t>PerfectoMobile</t>
-  </si>
-  <si>
     <t>cardExpiryMonth</t>
   </si>
   <si>
@@ -181,54 +178,21 @@
     <t>cardName</t>
   </si>
   <si>
-    <t>5163200000000008</t>
-  </si>
-  <si>
-    <t>070</t>
-  </si>
-  <si>
-    <t>2020</t>
-  </si>
-  <si>
-    <t>08-Aug</t>
-  </si>
-  <si>
-    <t>Srikanth</t>
-  </si>
-  <si>
-    <t>au.gov.nsw.onegov.MyLicences.uat</t>
-  </si>
-  <si>
     <t>appBuildName</t>
   </si>
   <si>
-    <t>2222</t>
-  </si>
-  <si>
-    <t>2-24 Rawson Pl,HAYMARKET,NSW 2000</t>
-  </si>
-  <si>
     <t>buildName</t>
   </si>
   <si>
     <t>UAT Checker</t>
   </si>
   <si>
-    <t>NSW Recreational Fishing Fee</t>
-  </si>
-  <si>
     <t>Empty</t>
   </si>
   <si>
     <t>windTunnelPersona</t>
   </si>
   <si>
-    <t>au.gov.nsw.onegov.app.holder.psm</t>
-  </si>
-  <si>
-    <t>Android</t>
-  </si>
-  <si>
     <t>PSM Holder</t>
   </si>
   <si>
@@ -238,15 +202,6 @@
     <t>test123</t>
   </si>
   <si>
-    <t>Guy Anthony CALLAGHAN</t>
-  </si>
-  <si>
-    <t>RO4128668</t>
-  </si>
-  <si>
-    <t>20 Oct 2015</t>
-  </si>
-  <si>
     <t>Alanna Scott</t>
   </si>
   <si>
@@ -265,18 +220,12 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>20 Oct 2016</t>
-  </si>
-  <si>
     <t>quickView_LicNum</t>
   </si>
   <si>
     <t>CCH######31</t>
   </si>
   <si>
-    <t>RO#####68</t>
-  </si>
-  <si>
     <t>quickView_LicStatus</t>
   </si>
   <si>
@@ -295,13 +244,7 @@
     <t>activity_EventType</t>
   </si>
   <si>
-    <t>Add</t>
-  </si>
-  <si>
-    <t>Recreational Fishing</t>
-  </si>
-  <si>
-    <t>Galaxy Note5</t>
+    <t>Firefox</t>
   </si>
 </sst>
 </file>
@@ -382,7 +325,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -666,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="B2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,21 +672,10 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E2" t="s">
-        <v>90</v>
-      </c>
-      <c r="K2" t="s">
-        <v>44</v>
-      </c>
-      <c r="L2" t="s">
-        <v>55</v>
-      </c>
-      <c r="M2" t="s">
-        <v>64</v>
-      </c>
+      <c r="J2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M2" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -753,10 +685,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W3"/>
+  <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="V9" sqref="V9"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -824,161 +756,92 @@
         <v>42</v>
       </c>
       <c r="M1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="O1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="N1" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="R1" s="6" t="s">
-        <v>56</v>
-      </c>
       <c r="S1" s="6" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="T1" s="5" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="U1" s="5" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="V1" s="5" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="W1" s="5" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>34</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J2" s="10">
         <v>2222</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="R2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="T2" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="U2" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="T2" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="U2" s="9" t="s">
-        <v>83</v>
-      </c>
       <c r="V2" s="7" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="W2" s="7" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="M3" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="N3" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="O3" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="P3" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q3" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="R3" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="T3" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="U3" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="V3" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="W3" s="7" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1"/>
-    <hyperlink ref="A2" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1046,10 +909,10 @@
         <v>31</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -1090,10 +953,10 @@
         <v>40</v>
       </c>
       <c r="M2" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="N2" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>